<commit_message>
Commercial sector demand update and documentation update
</commit_message>
<xml_diff>
--- a/TIMES-NZ/SubRES_TMPL/SubRES_NewTech_AGR_KEA_Trans.xlsx
+++ b/TIMES-NZ/SubRES_TMPL/SubRES_NewTech_AGR_KEA_Trans.xlsx
@@ -1,40 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\NZ_TIMES_model-v72.2\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weerasa\TIMES-NZ-Model-Files\TIMES-NZ\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07078184-DF4B-4BAC-933D-3EEFEC76ADD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AVA" sheetId="18" r:id="rId1"/>
-    <sheet name="AF_Trans" sheetId="17" r:id="rId2"/>
-    <sheet name="FILL Table" sheetId="19" r:id="rId3"/>
+    <sheet name="Documentation" sheetId="20" r:id="rId1"/>
+    <sheet name="AVA" sheetId="18" r:id="rId2"/>
+    <sheet name="AF_Trans" sheetId="17" r:id="rId3"/>
+    <sheet name="FILL Table" sheetId="19" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Amit Kanudia</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -64,13 +58,13 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Maurizio Gargiulo</author>
     <author>Gary Goldstein</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="1" shapeId="0">
+    <comment ref="I5" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -97,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N5" authorId="1" shapeId="0">
+    <comment ref="N5" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -115,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -217,12 +211,24 @@
   </si>
   <si>
     <t>AINDC-SH-Boiler-NGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Workbook: Mapping and transformation of new process in Agriculture, Forestry and Fishing Future Technologies across regions  for Kea Scenario </t>
+  </si>
+  <si>
+    <t>AVA: Process availability across regions</t>
+  </si>
+  <si>
+    <t>AF_Trans: Time-slice-specific availability factors for existing energy processes</t>
+  </si>
+  <si>
+    <t>FILL Table: Model data for transformation operations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -355,7 +361,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -371,24 +377,23 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="Comma 2" xfId="1"/>
+    <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="2"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 4" xfId="4"/>
-    <cellStyle name="Normal 4 2" xfId="5"/>
-    <cellStyle name="Normal 8" xfId="6"/>
-    <cellStyle name="Normal 9 2" xfId="7"/>
-    <cellStyle name="Normale_B2020" xfId="8"/>
-    <cellStyle name="Percent 2" xfId="9"/>
-    <cellStyle name="Percent 3" xfId="10"/>
-    <cellStyle name="Percent 4" xfId="11"/>
-    <cellStyle name="Standard_Sce_D_Extraction" xfId="12"/>
+    <cellStyle name="Normal 10" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 4" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 4 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 8" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 9 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normale_B2020" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Percent 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Percent 3" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Percent 4" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Standard_Sce_D_Extraction" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -404,9 +409,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -444,9 +449,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -481,7 +486,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -516,7 +521,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -689,28 +694,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24CB2892-F0CC-4065-A68A-8171F2DE7F2C}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7265625" customWidth="1"/>
+    <col min="2" max="2" width="31.81640625" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" ht="13" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
@@ -724,7 +764,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -732,7 +772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>33</v>
       </c>
@@ -740,7 +780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D16" s="11"/>
     </row>
   </sheetData>
@@ -749,8 +789,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:P15"/>
   <sheetViews>
@@ -758,34 +798,34 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" customWidth="1"/>
+    <col min="3" max="4" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.7265625" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.1796875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.85546875" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.81640625" customWidth="1"/>
+    <col min="18" max="18" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -798,7 +838,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="I6" s="2"/>
       <c r="J6" s="1"/>
@@ -809,7 +849,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
@@ -856,8 +896,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B8" s="12" t="s">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D8" t="s">
@@ -866,18 +906,18 @@
       <c r="E8">
         <v>2010</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="12">
         <v>0.4</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="12">
         <v>0.4</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B9" s="12" t="s">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
         <v>27</v>
       </c>
       <c r="D9" t="s">
@@ -886,18 +926,18 @@
       <c r="E9">
         <v>2010</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="12">
         <v>0.3</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="12">
         <v>0.35</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B10" s="12" t="s">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D10" t="s">
@@ -906,18 +946,18 @@
       <c r="E10">
         <v>2010</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="12">
         <v>0.42</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="12">
         <v>0.45</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B11" s="12" t="s">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D11" t="s">
@@ -929,15 +969,15 @@
       <c r="G11">
         <v>0.35</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="12">
         <v>0.3</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B12" s="12" t="s">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D12" t="s">
@@ -946,18 +986,18 @@
       <c r="E12">
         <v>2010</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="12">
         <v>0.35</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="12">
         <v>0.35</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B13" s="12" t="s">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
         <v>27</v>
       </c>
       <c r="D13" t="s">
@@ -966,18 +1006,18 @@
       <c r="E13">
         <v>2010</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="12">
         <v>0.25</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="12">
         <v>0.2</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B14" s="12" t="s">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D14" t="s">
@@ -986,18 +1026,18 @@
       <c r="E14">
         <v>2010</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="12">
         <v>0.3</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="12">
         <v>0.25</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B15" s="12" t="s">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D15" t="s">
@@ -1006,10 +1046,10 @@
       <c r="E15">
         <v>2010</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="12">
         <v>0.25</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="12">
         <v>0.2</v>
       </c>
       <c r="J15" s="11" t="s">
@@ -1025,37 +1065,37 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.7109375" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.54296875" customWidth="1"/>
+    <col min="2" max="2" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.7265625" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:14" ht="13" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>16</v>
       </c>

</xml_diff>